<commit_message>
clean requirements and add them to CRD client tests
</commit_message>
<xml_diff>
--- a/lib/davinci_crd_test_kit/requirements/cds-hooks-library_1.0.1_requirements.xlsx
+++ b/lib/davinci_crd_test_kit/requirements/cds-hooks-library_1.0.1_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlnaden/GlenViewAssociates/Inferno/source/davinci-crd-test-kit/lib/davinci_crd_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C377E1E-418F-7B42-9E5B-C7D3DAA425A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AF10EB-E13B-C94D-9836-96682E822072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Column Data" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$AH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirements!$A$1:$AH$94</definedName>
     <definedName name="EXPLODE" localSheetId="0">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="EXPLODE">_xlfn.LAMBDA(_xlpm.string,_xlfn.MAKEARRAY(1,LEN(_xlpm.string),_xlfn.LAMBDA(_xlpm.r,_xlpm.c,MID(_xlpm.string,_xlpm.c,1))))</definedName>
     <definedName name="FIND_DUPLICATES" localSheetId="0">_xlfn.LAMBDA(_xlpm.test_word,_xlpm.test_key,_xlpm.words,_xlpm.keys,_xlpm.threshold, _xlfn.LET(_xlpm.duplist,_xlfn._xlws.FILTER(_xlpm.keys,_xlfn.BYROW(_xlpm.words, _xlfn.LAMBDA(_xlpm.word, Info!HAMDIST(INDEX(_xlpm.word,1,1), _xlpm.test_word)&lt;_xlpm.threshold))),_xlfn.SINGLE(_xlfn._xlws.FILTER(_xlpm.duplist,_xlpm.duplist&lt;&gt;_xlpm.test_key,""))))</definedName>
@@ -2793,10 +2793,10 @@
   <dimension ref="A1:X94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4885,7 +4885,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH1" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}"/>
+  <autoFilter ref="A1:AH94" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B34" r:id="rId1" location="context" xr:uid="{2B58701D-4D03-4442-A640-91CB3237599B}"/>

</xml_diff>